<commit_message>
changed test .yml statuses to test_resource
</commit_message>
<xml_diff>
--- a/tests/data/ci_v2_data_exp.xlsx
+++ b/tests/data/ci_v2_data_exp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jedpreist/CodingStuff/DIMPACT/eam-core-provenance/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{621AB726-40B7-D04A-A727-CBFCBBB71CD3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15DE0F46-87E5-294F-A6F2-2DA62D969999}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="20960" windowHeight="16240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -225,10 +225,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="165" formatCode="0.00000"/>
     <numFmt numFmtId="166" formatCode="0.00000000000000000000000000000000000"/>
+    <numFmt numFmtId="188" formatCode="0.000000000000000000000000"/>
+    <numFmt numFmtId="207" formatCode="0.000000000000000000000E+00"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -383,7 +384,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -410,9 +411,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="188" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="207" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -797,13 +799,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="13.1640625" customWidth="1"/>
+    <col min="12" max="24" width="27.5" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="41.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1200,57 +1203,57 @@
       <c r="K10" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="L10" s="28">
-        <f>$F3*(1+$G3)^DATEDIF($J3,L8, "M")</f>
+      <c r="L10" s="27">
+        <f>$F3*(1+$G3)^(DATEDIF($J3,L8, "M") / 12)</f>
         <v>20</v>
       </c>
-      <c r="M10" s="28">
-        <f>$F3*(1+$G3)^DATEDIF($J3,M8, "M")</f>
+      <c r="M10" s="27">
+        <f t="shared" ref="M10:X10" si="1">$F3*(1+$G3)^(DATEDIF($J3,M8, "M") / 12)</f>
+        <v>21.189261887185907</v>
+      </c>
+      <c r="N10" s="27">
+        <f t="shared" si="1"/>
+        <v>22.44924096618746</v>
+      </c>
+      <c r="O10" s="27">
+        <f t="shared" si="1"/>
+        <v>23.78414230005442</v>
+      </c>
+      <c r="P10" s="27">
+        <f t="shared" si="1"/>
+        <v>25.198420997897465</v>
+      </c>
+      <c r="Q10" s="27">
+        <f t="shared" si="1"/>
+        <v>26.696797083400689</v>
+      </c>
+      <c r="R10" s="27">
+        <f t="shared" si="1"/>
+        <v>28.284271247461902</v>
+      </c>
+      <c r="S10" s="27">
+        <f t="shared" si="1"/>
+        <v>29.96614153753363</v>
+      </c>
+      <c r="T10" s="27">
+        <f t="shared" si="1"/>
+        <v>31.748021039363987</v>
+      </c>
+      <c r="U10" s="27">
+        <f t="shared" si="1"/>
+        <v>33.635856610148579</v>
+      </c>
+      <c r="V10" s="27">
+        <f t="shared" si="1"/>
+        <v>35.635948725613574</v>
+      </c>
+      <c r="W10" s="27">
+        <f t="shared" si="1"/>
+        <v>37.754972507267738</v>
+      </c>
+      <c r="X10" s="27">
+        <f t="shared" si="1"/>
         <v>40</v>
-      </c>
-      <c r="N10" s="28">
-        <f t="shared" ref="N10:V10" si="1">$F3*(1+$G3)^DATEDIF($J3,N8, "M")</f>
-        <v>80</v>
-      </c>
-      <c r="O10" s="28">
-        <f t="shared" si="1"/>
-        <v>160</v>
-      </c>
-      <c r="P10" s="28">
-        <f t="shared" si="1"/>
-        <v>320</v>
-      </c>
-      <c r="Q10" s="28">
-        <f t="shared" si="1"/>
-        <v>640</v>
-      </c>
-      <c r="R10" s="28">
-        <f t="shared" si="1"/>
-        <v>1280</v>
-      </c>
-      <c r="S10" s="28">
-        <f t="shared" si="1"/>
-        <v>2560</v>
-      </c>
-      <c r="T10" s="28">
-        <f t="shared" si="1"/>
-        <v>5120</v>
-      </c>
-      <c r="U10" s="28">
-        <f t="shared" si="1"/>
-        <v>10240</v>
-      </c>
-      <c r="V10" s="28">
-        <f t="shared" si="1"/>
-        <v>20480</v>
-      </c>
-      <c r="W10" s="28">
-        <f>$F3*(1+$G3)^DATEDIF($J3,W8, "M")</f>
-        <v>40960</v>
-      </c>
-      <c r="X10" s="28">
-        <f>$F3*(1+$G3)^DATEDIF($J3,X8, "M")</f>
-        <v>81920</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
@@ -1485,61 +1488,61 @@
       <c r="K15" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="L15" s="26">
+      <c r="L15" s="28">
         <f>L9*$F10*L10*$F11*$F13</f>
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="M15" s="16">
+      <c r="M15" s="28">
         <f t="shared" ref="M15:X15" si="5">M9*$F10*M10*$F11*$F13</f>
+        <v>2.118926188718591E-4</v>
+      </c>
+      <c r="N15" s="28">
+        <f t="shared" si="5"/>
+        <v>2.2449240966187462E-4</v>
+      </c>
+      <c r="O15" s="28">
+        <f t="shared" si="5"/>
+        <v>2.3784142300054421E-4</v>
+      </c>
+      <c r="P15" s="28">
+        <f t="shared" si="5"/>
+        <v>2.5198420997897466E-4</v>
+      </c>
+      <c r="Q15" s="28">
+        <f t="shared" si="5"/>
+        <v>2.6696797083400694E-4</v>
+      </c>
+      <c r="R15" s="28">
+        <f t="shared" si="5"/>
+        <v>2.8284271247461907E-4</v>
+      </c>
+      <c r="S15" s="28">
+        <f t="shared" si="5"/>
+        <v>2.9966141537533634E-4</v>
+      </c>
+      <c r="T15" s="28">
+        <f t="shared" si="5"/>
+        <v>3.1748021039363988E-4</v>
+      </c>
+      <c r="U15" s="28">
+        <f t="shared" si="5"/>
+        <v>3.3635856610148582E-4</v>
+      </c>
+      <c r="V15" s="28">
+        <f t="shared" si="5"/>
+        <v>3.5635948725613577E-4</v>
+      </c>
+      <c r="W15" s="28">
+        <f t="shared" si="5"/>
+        <v>3.7754972507267738E-4</v>
+      </c>
+      <c r="X15" s="28">
+        <f t="shared" si="5"/>
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="N15" s="16">
-        <f t="shared" si="5"/>
-        <v>8.0000000000000004E-4</v>
-      </c>
-      <c r="O15" s="16">
-        <f t="shared" si="5"/>
-        <v>1.6000000000000001E-3</v>
-      </c>
-      <c r="P15" s="16">
-        <f t="shared" si="5"/>
-        <v>3.2000000000000002E-3</v>
-      </c>
-      <c r="Q15" s="16">
-        <f t="shared" si="5"/>
-        <v>6.4000000000000003E-3</v>
-      </c>
-      <c r="R15" s="16">
-        <f t="shared" si="5"/>
-        <v>1.2800000000000001E-2</v>
-      </c>
-      <c r="S15" s="16">
-        <f t="shared" si="5"/>
-        <v>2.5600000000000001E-2</v>
-      </c>
-      <c r="T15" s="16">
-        <f t="shared" si="5"/>
-        <v>5.1200000000000002E-2</v>
-      </c>
-      <c r="U15" s="16">
-        <f t="shared" si="5"/>
-        <v>0.1024</v>
-      </c>
-      <c r="V15" s="16">
-        <f t="shared" si="5"/>
-        <v>0.20480000000000001</v>
-      </c>
-      <c r="W15" s="16">
-        <f t="shared" si="5"/>
-        <v>0.40960000000000002</v>
-      </c>
-      <c r="X15" s="16">
-        <f t="shared" si="5"/>
-        <v>0.81920000000000004</v>
-      </c>
-      <c r="Z15" s="27">
+      <c r="Z15" s="26">
         <f>SUM(L15:X15)</f>
-        <v>1.6381999999999999</v>
+        <v>3.7634307490211532E-3</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
@@ -1552,51 +1555,51 @@
       </c>
       <c r="M16" s="24">
         <f t="shared" ref="M16:X16" si="6">M10*M12*$F12</f>
-        <v>5.0000000000000001E-3</v>
+        <v>2.6486577358982386E-3</v>
       </c>
       <c r="N16" s="24">
         <f t="shared" si="6"/>
-        <v>0.01</v>
+        <v>2.8061551207734323E-3</v>
       </c>
       <c r="O16" s="24">
         <f t="shared" si="6"/>
-        <v>0.02</v>
+        <v>2.9730177875068025E-3</v>
       </c>
       <c r="P16" s="24">
         <f t="shared" si="6"/>
-        <v>0.04</v>
+        <v>3.1498026247371832E-3</v>
       </c>
       <c r="Q16" s="24">
         <f t="shared" si="6"/>
-        <v>0.08</v>
+        <v>3.3370996354250863E-3</v>
       </c>
       <c r="R16" s="24">
         <f t="shared" si="6"/>
-        <v>0.16</v>
+        <v>3.5355339059327381E-3</v>
       </c>
       <c r="S16" s="24">
         <f t="shared" si="6"/>
-        <v>0.32</v>
+        <v>3.7457676921917038E-3</v>
       </c>
       <c r="T16" s="24">
         <f t="shared" si="6"/>
-        <v>0.64</v>
+        <v>3.9685026299204991E-3</v>
       </c>
       <c r="U16" s="24">
         <f t="shared" si="6"/>
-        <v>1.28</v>
+        <v>4.2044820762685729E-3</v>
       </c>
       <c r="V16" s="24">
         <f t="shared" si="6"/>
-        <v>2.56</v>
+        <v>4.4544935907016971E-3</v>
       </c>
       <c r="W16" s="24">
         <f t="shared" si="6"/>
-        <v>5.12</v>
+        <v>4.7193715634084674E-3</v>
       </c>
       <c r="X16" s="24">
         <f t="shared" si="6"/>
-        <v>10.24</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="17" spans="2:26" x14ac:dyDescent="0.2">
@@ -1644,61 +1647,61 @@
       <c r="K18" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="L18" s="24">
+      <c r="L18" s="29">
         <f>L16*L11*$F13*$F14</f>
         <v>4.9999999999999998E-8</v>
       </c>
-      <c r="M18" s="24">
+      <c r="M18" s="29">
         <f t="shared" ref="M18:X18" si="7">M16*M11*$F13*$F14</f>
+        <v>5.297315471796477E-8</v>
+      </c>
+      <c r="N18" s="29">
+        <f t="shared" si="7"/>
+        <v>5.6123102415468647E-8</v>
+      </c>
+      <c r="O18" s="29">
+        <f t="shared" si="7"/>
+        <v>5.9460355750136046E-8</v>
+      </c>
+      <c r="P18" s="29">
+        <f t="shared" si="7"/>
+        <v>6.2996052494743653E-8</v>
+      </c>
+      <c r="Q18" s="29">
+        <f t="shared" si="7"/>
+        <v>6.6741992708501728E-8</v>
+      </c>
+      <c r="R18" s="29">
+        <f t="shared" si="7"/>
+        <v>7.0710678118654758E-8</v>
+      </c>
+      <c r="S18" s="29">
+        <f t="shared" si="7"/>
+        <v>7.4915353843834077E-8</v>
+      </c>
+      <c r="T18" s="29">
+        <f t="shared" si="7"/>
+        <v>7.9370052598409976E-8</v>
+      </c>
+      <c r="U18" s="29">
+        <f t="shared" si="7"/>
+        <v>8.408964152537146E-8</v>
+      </c>
+      <c r="V18" s="29">
+        <f t="shared" si="7"/>
+        <v>8.9089871814033941E-8</v>
+      </c>
+      <c r="W18" s="29">
+        <f t="shared" si="7"/>
+        <v>9.4387431268169333E-8</v>
+      </c>
+      <c r="X18" s="29">
+        <f t="shared" si="7"/>
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="N18" s="24">
-        <f t="shared" si="7"/>
-        <v>1.9999999999999999E-7</v>
-      </c>
-      <c r="O18" s="24">
-        <f t="shared" si="7"/>
-        <v>3.9999999999999998E-7</v>
-      </c>
-      <c r="P18" s="24">
-        <f t="shared" si="7"/>
-        <v>7.9999999999999996E-7</v>
-      </c>
-      <c r="Q18" s="24">
-        <f t="shared" si="7"/>
-        <v>1.5999999999999999E-6</v>
-      </c>
-      <c r="R18" s="24">
-        <f t="shared" si="7"/>
-        <v>3.1999999999999999E-6</v>
-      </c>
-      <c r="S18" s="24">
-        <f t="shared" si="7"/>
-        <v>6.3999999999999997E-6</v>
-      </c>
-      <c r="T18" s="24">
-        <f t="shared" si="7"/>
-        <v>1.2799999999999999E-5</v>
-      </c>
-      <c r="U18" s="24">
-        <f t="shared" si="7"/>
-        <v>2.5599999999999999E-5</v>
-      </c>
-      <c r="V18" s="24">
-        <f t="shared" si="7"/>
-        <v>5.1199999999999998E-5</v>
-      </c>
-      <c r="W18" s="24">
-        <f t="shared" si="7"/>
-        <v>1.024E-4</v>
-      </c>
-      <c r="X18" s="24">
-        <f t="shared" si="7"/>
-        <v>2.0479999999999999E-4</v>
-      </c>
-      <c r="Z18" s="27">
+      <c r="Z18" s="26">
         <f>SUM(L18:X18)</f>
-        <v>4.0954999999999995E-4</v>
+        <v>9.4085768725528831E-7</v>
       </c>
     </row>
     <row r="19" spans="2:26" x14ac:dyDescent="0.2">
@@ -1731,51 +1734,51 @@
       </c>
       <c r="M19" s="24">
         <f t="shared" ref="M19:X19" si="8">M16</f>
-        <v>5.0000000000000001E-3</v>
+        <v>2.6486577358982386E-3</v>
       </c>
       <c r="N19" s="24">
         <f t="shared" si="8"/>
-        <v>0.01</v>
+        <v>2.8061551207734323E-3</v>
       </c>
       <c r="O19" s="24">
         <f t="shared" si="8"/>
-        <v>0.02</v>
+        <v>2.9730177875068025E-3</v>
       </c>
       <c r="P19" s="24">
         <f t="shared" si="8"/>
-        <v>0.04</v>
+        <v>3.1498026247371832E-3</v>
       </c>
       <c r="Q19" s="24">
         <f t="shared" si="8"/>
-        <v>0.08</v>
+        <v>3.3370996354250863E-3</v>
       </c>
       <c r="R19" s="24">
         <f t="shared" si="8"/>
-        <v>0.16</v>
+        <v>3.5355339059327381E-3</v>
       </c>
       <c r="S19" s="24">
         <f t="shared" si="8"/>
-        <v>0.32</v>
+        <v>3.7457676921917038E-3</v>
       </c>
       <c r="T19" s="24">
         <f t="shared" si="8"/>
-        <v>0.64</v>
+        <v>3.9685026299204991E-3</v>
       </c>
       <c r="U19" s="24">
         <f t="shared" si="8"/>
-        <v>1.28</v>
+        <v>4.2044820762685729E-3</v>
       </c>
       <c r="V19" s="24">
         <f t="shared" si="8"/>
-        <v>2.56</v>
+        <v>4.4544935907016971E-3</v>
       </c>
       <c r="W19" s="24">
         <f t="shared" si="8"/>
-        <v>5.12</v>
+        <v>4.7193715634084674E-3</v>
       </c>
       <c r="X19" s="24">
         <f t="shared" si="8"/>
-        <v>10.24</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="20" spans="2:26" x14ac:dyDescent="0.2">
@@ -1808,55 +1811,55 @@
       </c>
       <c r="M21" s="24">
         <f t="shared" ref="M21:X21" si="9">M19*M11*$F14*$F13</f>
-        <v>9.9999999999999995E-8</v>
+        <v>5.297315471796477E-8</v>
       </c>
       <c r="N21" s="24">
         <f t="shared" si="9"/>
-        <v>1.9999999999999999E-7</v>
+        <v>5.6123102415468647E-8</v>
       </c>
       <c r="O21" s="24">
         <f t="shared" si="9"/>
-        <v>3.9999999999999998E-7</v>
+        <v>5.9460355750136046E-8</v>
       </c>
       <c r="P21" s="24">
         <f t="shared" si="9"/>
-        <v>7.9999999999999996E-7</v>
+        <v>6.2996052494743653E-8</v>
       </c>
       <c r="Q21" s="24">
         <f t="shared" si="9"/>
-        <v>1.5999999999999999E-6</v>
+        <v>6.6741992708501728E-8</v>
       </c>
       <c r="R21" s="24">
         <f t="shared" si="9"/>
-        <v>3.1999999999999999E-6</v>
+        <v>7.0710678118654758E-8</v>
       </c>
       <c r="S21" s="24">
         <f t="shared" si="9"/>
-        <v>6.3999999999999997E-6</v>
+        <v>7.4915353843834077E-8</v>
       </c>
       <c r="T21" s="24">
         <f t="shared" si="9"/>
-        <v>1.2799999999999999E-5</v>
+        <v>7.9370052598409976E-8</v>
       </c>
       <c r="U21" s="24">
         <f t="shared" si="9"/>
-        <v>2.5599999999999999E-5</v>
+        <v>8.408964152537146E-8</v>
       </c>
       <c r="V21" s="24">
         <f t="shared" si="9"/>
-        <v>5.1199999999999998E-5</v>
+        <v>8.9089871814033941E-8</v>
       </c>
       <c r="W21" s="24">
         <f t="shared" si="9"/>
-        <v>1.024E-4</v>
+        <v>9.4387431268169333E-8</v>
       </c>
       <c r="X21" s="24">
         <f t="shared" si="9"/>
-        <v>2.0479999999999999E-4</v>
-      </c>
-      <c r="Z21" s="27">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="Z21" s="26">
         <f>SUM(L21:X21)</f>
-        <v>4.0954999999999995E-4</v>
+        <v>9.4085768725528831E-7</v>
       </c>
     </row>
     <row r="22" spans="2:26" x14ac:dyDescent="0.2">

</xml_diff>